<commit_message>
:hammer: Updating screw sizes at the part list
</commit_message>
<xml_diff>
--- a/Part Sizes and Parts list.xlsx
+++ b/Part Sizes and Parts list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Everymind\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\pessoal\OpenSCAD\Sigma_Soldering_Booth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942CD3EF-7EC6-43F4-866F-0EC87B362278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC70787C-E51B-4588-A7F7-9FA1665FE171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rought cut part size" sheetId="1" r:id="rId1"/>
@@ -258,27 +258,18 @@
     <t>Screws for wood</t>
   </si>
   <si>
-    <t>3,5 x 5</t>
-  </si>
-  <si>
     <t>MWS</t>
   </si>
   <si>
     <t>Medium wooden screws</t>
   </si>
   <si>
-    <t>3,5 x 25</t>
-  </si>
-  <si>
     <t>BWS</t>
   </si>
   <si>
     <t>Big wooden screws</t>
   </si>
   <si>
-    <t>3,5 x 50</t>
-  </si>
-  <si>
     <t>WG</t>
   </si>
   <si>
@@ -295,6 +286,15 @@
   </si>
   <si>
     <t>Silicone sealant</t>
+  </si>
+  <si>
+    <t>M3 x 8mm</t>
+  </si>
+  <si>
+    <t>M3 x 25 mm</t>
+  </si>
+  <si>
+    <t>M3 x 50 mm</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1385,45 +1385,78 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1431,35 +1464,11 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1469,24 +1478,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1724,7 +1715,7 @@
   </sheetPr>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1753,28 +1744,28 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="122" t="s">
+      <c r="B2" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="123"/>
-      <c r="D2" s="124"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="142"/>
       <c r="E2" s="3"/>
       <c r="F2" s="4"/>
-      <c r="G2" s="125" t="s">
+      <c r="G2" s="121" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="127"/>
+      <c r="H2" s="122"/>
+      <c r="I2" s="122"/>
+      <c r="J2" s="123"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="128" t="s">
+      <c r="B3" s="124" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="129"/>
-      <c r="D3" s="130"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="126"/>
       <c r="E3" s="1"/>
       <c r="F3" s="5"/>
       <c r="G3" s="6" t="s">
@@ -1796,12 +1787,12 @@
       <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="131">
+      <c r="C4" s="127">
         <v>450</v>
       </c>
-      <c r="D4" s="132"/>
+      <c r="D4" s="128"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="133" t="s">
+      <c r="F4" s="129" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="9" t="s">
@@ -1826,12 +1817,12 @@
       <c r="B5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="134">
+      <c r="C5" s="133">
         <v>900</v>
       </c>
-      <c r="D5" s="135"/>
+      <c r="D5" s="134"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="120"/>
+      <c r="F5" s="130"/>
       <c r="G5" s="14" t="s">
         <v>9</v>
       </c>
@@ -1854,12 +1845,12 @@
       <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="131">
+      <c r="C6" s="127">
         <v>150</v>
       </c>
-      <c r="D6" s="132"/>
+      <c r="D6" s="128"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="119"/>
+      <c r="F6" s="131"/>
       <c r="G6" s="18" t="s">
         <v>10</v>
       </c>
@@ -1882,12 +1873,12 @@
       <c r="B7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="114" t="s">
+      <c r="C7" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="115"/>
+      <c r="D7" s="136"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="120"/>
+      <c r="F7" s="130"/>
       <c r="G7" s="14" t="s">
         <v>13</v>
       </c>
@@ -1910,12 +1901,12 @@
       <c r="B8" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="117"/>
+      <c r="D8" s="138"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="121"/>
+      <c r="F8" s="132"/>
       <c r="G8" s="24" t="s">
         <v>16</v>
       </c>
@@ -1939,7 +1930,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="118" t="s">
+      <c r="F9" s="139" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="14" t="s">
@@ -1971,7 +1962,7 @@
         <v>21</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="119"/>
+      <c r="F10" s="131"/>
       <c r="G10" s="18" t="s">
         <v>22</v>
       </c>
@@ -2002,7 +1993,7 @@
         <v>5</v>
       </c>
       <c r="E11" s="35"/>
-      <c r="F11" s="120"/>
+      <c r="F11" s="130"/>
       <c r="G11" s="14" t="s">
         <v>24</v>
       </c>
@@ -2033,7 +2024,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="35"/>
-      <c r="F12" s="121"/>
+      <c r="F12" s="132"/>
       <c r="G12" s="24" t="s">
         <v>26</v>
       </c>
@@ -2064,7 +2055,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="35"/>
-      <c r="F13" s="118" t="s">
+      <c r="F13" s="139" t="s">
         <v>28</v>
       </c>
       <c r="G13" s="14" t="s">
@@ -2097,7 +2088,7 @@
         <v>1</v>
       </c>
       <c r="E14" s="35"/>
-      <c r="F14" s="119"/>
+      <c r="F14" s="131"/>
       <c r="G14" s="18" t="s">
         <v>31</v>
       </c>
@@ -2128,7 +2119,7 @@
         <v>50</v>
       </c>
       <c r="E15" s="35"/>
-      <c r="F15" s="120"/>
+      <c r="F15" s="130"/>
       <c r="G15" s="41" t="s">
         <v>33</v>
       </c>
@@ -2158,7 +2149,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="1"/>
-      <c r="F16" s="119"/>
+      <c r="F16" s="131"/>
       <c r="G16" s="47" t="s">
         <v>36</v>
       </c>
@@ -2189,7 +2180,7 @@
         <v>Millimeters</v>
       </c>
       <c r="E17" s="1"/>
-      <c r="F17" s="120"/>
+      <c r="F17" s="130"/>
       <c r="G17" s="51" t="s">
         <v>38</v>
       </c>
@@ -2239,6 +2230,9 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F9:F12"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -2247,9 +2241,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F9:F12"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:D8">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -2280,7 +2271,9 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2324,14 +2317,14 @@
       <c r="D2" s="64" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="136" t="str">
+      <c r="E2" s="143" t="str">
         <f>_xlfn.CONCAT("Dimention (",_xlfn.CONCAT(_xlfn.CONCAT("in ",'Rought cut part size'!C8),")"))</f>
         <v>Dimention (in Millimeters)</v>
       </c>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="138"/>
+      <c r="F2" s="144"/>
+      <c r="G2" s="144"/>
+      <c r="H2" s="144"/>
+      <c r="I2" s="145"/>
       <c r="J2" s="65" t="s">
         <v>43</v>
       </c>
@@ -2947,10 +2940,10 @@
       <c r="J18" s="87">
         <v>2</v>
       </c>
-      <c r="K18" s="139" t="s">
+      <c r="K18" s="146" t="s">
         <v>68</v>
       </c>
-      <c r="L18" s="140"/>
+      <c r="L18" s="147"/>
       <c r="M18" s="79"/>
     </row>
     <row r="19" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
@@ -2966,22 +2959,22 @@
       </c>
       <c r="E19" s="99"/>
       <c r="F19" s="100"/>
-      <c r="G19" s="101" t="s">
-        <v>72</v>
+      <c r="G19" s="100" t="s">
+        <v>82</v>
       </c>
       <c r="H19" s="100"/>
-      <c r="I19" s="102"/>
-      <c r="J19" s="103">
+      <c r="I19" s="101"/>
+      <c r="J19" s="102">
         <f>CEILING((((G17*J17)+(G18*J18))/
 IF('Rought cut part size'!C8='Rought cut part size'!C17,1000,
 IF('Rought cut part size'!C8='Rought cut part size'!C18,100,1))*L19),1)</f>
         <v>36</v>
       </c>
-      <c r="K19" s="104" t="str">
+      <c r="K19" s="103" t="str">
         <f>_xlfn.CONCAT(_xlfn.CONCAT("Screws/",IF('Rought cut part size'!C7='Rought cut part size'!B16,#REF!,IF('Rought cut part size'!C8='Rought cut part size'!C17,"1000mm","100cm"))),":")</f>
         <v>Screws/1000mm:</v>
       </c>
-      <c r="L19" s="105">
+      <c r="L19" s="104">
         <v>10</v>
       </c>
       <c r="M19" s="79"/>
@@ -2989,21 +2982,21 @@
     <row r="20" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="94" t="s">
         <v>73</v>
-      </c>
-      <c r="C20" s="94" t="s">
-        <v>74</v>
       </c>
       <c r="D20" s="82" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="106"/>
-      <c r="F20" s="107"/>
-      <c r="G20" s="108" t="s">
-        <v>75</v>
-      </c>
-      <c r="H20" s="107"/>
-      <c r="I20" s="109"/>
+      <c r="E20" s="105"/>
+      <c r="F20" s="106"/>
+      <c r="G20" s="106" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" s="106"/>
+      <c r="I20" s="107"/>
       <c r="J20" s="87">
         <v>8</v>
       </c>
@@ -3018,21 +3011,21 @@
     <row r="21" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="69" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C21" s="89" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D21" s="71" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="110"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="112" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="111"/>
-      <c r="I21" s="113"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="109"/>
+      <c r="I21" s="110"/>
       <c r="J21" s="76">
         <v>8</v>
       </c>
@@ -3047,23 +3040,23 @@
     <row r="22" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="80" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C22" s="94" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="141" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="145"/>
-      <c r="F22" s="142"/>
-      <c r="G22" s="142" t="s">
-        <v>49</v>
-      </c>
-      <c r="H22" s="142"/>
-      <c r="I22" s="143"/>
+        <v>77</v>
+      </c>
+      <c r="D22" s="111" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="115"/>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="112"/>
+      <c r="I22" s="113"/>
       <c r="J22" s="87" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K22" s="77" t="s">
         <v>49</v>
@@ -3076,23 +3069,23 @@
     <row r="23" spans="1:13" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="69" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="149" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="144" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="146"/>
-      <c r="F23" s="147"/>
-      <c r="G23" s="150" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" s="147"/>
-      <c r="I23" s="148"/>
+        <v>80</v>
+      </c>
+      <c r="C23" s="119" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="114" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="116"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="120" t="s">
+        <v>49</v>
+      </c>
+      <c r="H23" s="117"/>
+      <c r="I23" s="118"/>
       <c r="J23" s="87" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="K23" s="79" t="s">
         <v>49</v>

</xml_diff>